<commit_message>
Replace Methodology Decision Tool
</commit_message>
<xml_diff>
--- a/static/ms-office/Methodology_Decision_Tool.xlsx
+++ b/static/ms-office/Methodology_Decision_Tool.xlsx
@@ -19,12 +19,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Aspect</t>
-  </si>
-  <si>
-    <t>Considering Mode 1</t>
-  </si>
-  <si>
-    <t>Considering Mode 2</t>
   </si>
   <si>
     <t>"Ready.  Aim.  Aim.  Fire."</t>
@@ -84,9 +78,6 @@
     <t xml:space="preserve">small-number weightings are relative to other aspects in the vertical (mode) </t>
   </si>
   <si>
-    <t>This compares bimodality, and indicates a preference, though outliers below must be addressed</t>
-  </si>
-  <si>
     <t>“institutional”, legacy, predictable, familiar, hardware</t>
   </si>
   <si>
@@ -120,14 +111,23 @@
     <t>Implementation Algorithm…</t>
   </si>
   <si>
-    <t>OCIO Methodology Decision Tool</t>
+    <t>This compares modality, and indicates a preference, though outliers below must be addressed</t>
+  </si>
+  <si>
+    <t>Considering Mode 1 (Waterfall)</t>
+  </si>
+  <si>
+    <t>Considering Mode 2 (Agile)</t>
+  </si>
+  <si>
+    <t>Methodology Decision Tool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +187,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -477,9 +491,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -511,34 +522,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -564,25 +565,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE30"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25:Y25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,605 +929,606 @@
     <col min="28" max="28" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+    <row r="1" spans="1:31" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
     </row>
-    <row r="2" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
+    <row r="2" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
     </row>
-    <row r="3" spans="2:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AA3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC3" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="43"/>
+    <row r="3" spans="1:31" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="38"/>
     </row>
-    <row r="4" spans="2:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+    <row r="4" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="AA4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="39"/>
+      <c r="AE4" s="40"/>
+    </row>
+    <row r="5" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="53"/>
+      <c r="AA5" s="16">
+        <f>SUM(AA7:AA25)</f>
+        <v>-3.3000000000000012</v>
+      </c>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="42"/>
+    </row>
+    <row r="6" spans="1:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="AA4" s="22" t="s">
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="45"/>
-    </row>
-    <row r="5" spans="2:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="51"/>
-      <c r="AA5" s="17">
-        <f>SUM(AA7:AA25)</f>
-        <v>39.000000000000007</v>
-      </c>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="47"/>
-    </row>
-    <row r="6" spans="2:31" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
       <c r="Z6" s="7"/>
-      <c r="AA6" s="12"/>
+      <c r="AA6" s="11"/>
       <c r="AD6" s="4"/>
     </row>
-    <row r="7" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
-      <c r="C7" s="37">
+      <c r="C7" s="31">
         <v>2</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="19">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O7" s="52">
-        <v>8</v>
-      </c>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="53"/>
-      <c r="W7" s="53"/>
-      <c r="X7" s="53"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="19">
+      <c r="O7" s="28">
+        <v>3</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="18">
         <v>1.3</v>
       </c>
-      <c r="AA7" s="12">
+      <c r="AA7" s="11">
         <f>O7*N7-C7*Z7</f>
-        <v>6.2000000000000011</v>
-      </c>
-      <c r="AC7" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD7" s="40"/>
-      <c r="AE7" s="40"/>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="AC7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="35"/>
     </row>
-    <row r="8" spans="2:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
-      <c r="N8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="12"/>
-      <c r="AC8" s="40"/>
-      <c r="AD8" s="40"/>
-      <c r="AE8" s="40"/>
+      <c r="N8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="11"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
     </row>
-    <row r="9" spans="2:31" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="11"/>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="31">
+        <v>4</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="O10" s="31">
+        <v>2</v>
+      </c>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="AA10" s="11">
+        <f>O10*N10-C10*Z10</f>
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="N11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="11"/>
+    </row>
+    <row r="12" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="11"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="31">
+        <v>6</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="O13" s="31">
+        <v>3</v>
+      </c>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="18">
+        <v>1.6</v>
+      </c>
+      <c r="AA13" s="11">
+        <f>O13*Z13-C13*N13</f>
+        <v>-4.8000000000000007</v>
+      </c>
+      <c r="AB13" s="9"/>
+    </row>
+    <row r="14" spans="1:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="N14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="9"/>
+    </row>
+    <row r="15" spans="1:31" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="50"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="50"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="12"/>
+      <c r="C15" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="11"/>
     </row>
-    <row r="10" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="37">
-        <v>8</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="19">
-        <v>1.6</v>
-      </c>
-      <c r="O10" s="37">
-        <v>5</v>
-      </c>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="19">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C16" s="31">
+        <v>1</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="18">
         <v>1.5</v>
       </c>
-      <c r="AA10" s="12">
-        <f>O10*N10-C10*Z10</f>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="N11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="12"/>
-    </row>
-    <row r="12" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="48"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="12"/>
-    </row>
-    <row r="13" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="37">
-        <v>1</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="19">
-        <v>1.6</v>
-      </c>
-      <c r="O13" s="37">
-        <v>9</v>
-      </c>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="39"/>
-      <c r="Z13" s="19">
-        <v>1.6</v>
-      </c>
-      <c r="AA13" s="12">
-        <f>O13*Z13-C13*N13</f>
-        <v>12.8</v>
-      </c>
-      <c r="AB13" s="10"/>
-    </row>
-    <row r="14" spans="2:31" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="N14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="10"/>
-    </row>
-    <row r="15" spans="2:31" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="12"/>
-    </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="C16" s="37">
-        <v>1</v>
-      </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="O16" s="37">
-        <v>9</v>
-      </c>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="38"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="38"/>
-      <c r="V16" s="38"/>
-      <c r="W16" s="38"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="39"/>
-      <c r="Z16" s="20">
+      <c r="O16" s="31">
+        <v>3</v>
+      </c>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="19">
         <v>1.4</v>
       </c>
-      <c r="AA16" s="12">
+      <c r="AA16" s="11">
         <f>(O16*N16-C16*Z16)</f>
-        <v>12.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N17" s="9"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="12"/>
+      <c r="N17" s="8"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="11"/>
     </row>
     <row r="18" spans="2:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="11"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C19" s="52">
+      <c r="C19" s="28">
         <v>2</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="19">
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="18">
         <v>1.4</v>
       </c>
-      <c r="O19" s="52">
-        <v>6</v>
-      </c>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="54"/>
-      <c r="Z19" s="20">
+      <c r="O19" s="28">
+        <v>3</v>
+      </c>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="30"/>
+      <c r="Z19" s="19">
         <v>1.5</v>
       </c>
-      <c r="AA19" s="12">
+      <c r="AA19" s="11">
         <f>(O19*Z19-C19*N19)</f>
-        <v>6.2</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="20" spans="2:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N20" s="6"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="12"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="11"/>
     </row>
     <row r="21" spans="2:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="49"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
       <c r="Z21" s="6"/>
-      <c r="AA21" s="12"/>
+      <c r="AA21" s="11"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C22" s="37">
+      <c r="C22" s="31">
         <v>3</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="19">
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="18">
         <v>1</v>
       </c>
-      <c r="O22" s="37">
+      <c r="O22" s="31">
         <v>3</v>
       </c>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="38"/>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="39"/>
-      <c r="Z22" s="19">
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="18">
         <v>1.7</v>
       </c>
-      <c r="AA22" s="12">
+      <c r="AA22" s="11">
         <f>O22*Z22-C22*N22</f>
         <v>2.0999999999999996</v>
       </c>
@@ -1517,195 +1536,218 @@
     <row r="23" spans="2:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N23" s="6"/>
       <c r="Z23" s="6"/>
-      <c r="AA23" s="12"/>
+      <c r="AA23" s="11"/>
     </row>
     <row r="24" spans="2:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
+        <v>10</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="48"/>
+      <c r="O24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
       <c r="Z24" s="6"/>
-      <c r="AA24" s="12"/>
+      <c r="AA24" s="11"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C25" s="37">
+      <c r="C25" s="31">
+        <v>6</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="18">
+        <v>1.3</v>
+      </c>
+      <c r="O25" s="31">
         <v>3</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="19">
-        <v>1.3</v>
-      </c>
-      <c r="O25" s="37">
-        <v>5</v>
-      </c>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="38"/>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="39"/>
-      <c r="Z25" s="19">
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="33"/>
+      <c r="Z25" s="18">
         <v>1.5</v>
       </c>
-      <c r="AA25" s="12">
+      <c r="AA25" s="11">
         <f>O25*Z25-C25*N25</f>
-        <v>3.5999999999999996</v>
+        <v>-3.3000000000000007</v>
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="AA26" s="13"/>
+      <c r="AA26" s="12"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C27" s="32">
+      <c r="C27" s="50">
         <f>C7*N7+C10*N10+C13*N13+C16*N16+C19*N19+C22*N22+C25*N25</f>
-        <v>27.800000000000004</v>
-      </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="34"/>
-      <c r="O27" s="32">
+        <v>33.300000000000004</v>
+      </c>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="52"/>
+      <c r="O27" s="50">
         <f>O7*Z7+O10*Z10+O13*Z13+O16*Z16+O19*Z19+O22*Z22+O25*Z25</f>
-        <v>66.5</v>
-      </c>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="52"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C28" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
-      <c r="O28" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="25"/>
+      <c r="C28" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="24"/>
+      <c r="O28" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="24"/>
     </row>
     <row r="29" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="46"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="21"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="F29:W30"/>
+    <mergeCell ref="C27:M27"/>
+    <mergeCell ref="O27:Y27"/>
+    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="O4:Y4"/>
+    <mergeCell ref="C25:M25"/>
+    <mergeCell ref="O25:Y25"/>
+    <mergeCell ref="AC7:AE8"/>
+    <mergeCell ref="AC3:AE5"/>
+    <mergeCell ref="C24:M24"/>
+    <mergeCell ref="O24:Y24"/>
+    <mergeCell ref="C21:M21"/>
+    <mergeCell ref="O21:Y21"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="O22:Y22"/>
+    <mergeCell ref="O10:Y10"/>
+    <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="O5:Y5"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C7:M7"/>
+    <mergeCell ref="O7:Y7"/>
+    <mergeCell ref="O6:Y6"/>
     <mergeCell ref="C2:Z2"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="C18:M18"/>
@@ -1722,29 +1764,6 @@
     <mergeCell ref="C9:M9"/>
     <mergeCell ref="O9:Y9"/>
     <mergeCell ref="C10:M10"/>
-    <mergeCell ref="AC7:AE8"/>
-    <mergeCell ref="AC3:AE5"/>
-    <mergeCell ref="C24:M24"/>
-    <mergeCell ref="O24:Y24"/>
-    <mergeCell ref="C21:M21"/>
-    <mergeCell ref="O21:Y21"/>
-    <mergeCell ref="C22:M22"/>
-    <mergeCell ref="O22:Y22"/>
-    <mergeCell ref="O10:Y10"/>
-    <mergeCell ref="C12:M12"/>
-    <mergeCell ref="C5:M5"/>
-    <mergeCell ref="O5:Y5"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C7:M7"/>
-    <mergeCell ref="O7:Y7"/>
-    <mergeCell ref="O6:Y6"/>
-    <mergeCell ref="F29:W30"/>
-    <mergeCell ref="C27:M27"/>
-    <mergeCell ref="O27:Y27"/>
-    <mergeCell ref="C4:M4"/>
-    <mergeCell ref="O4:Y4"/>
-    <mergeCell ref="C25:M25"/>
-    <mergeCell ref="O25:Y25"/>
   </mergeCells>
   <conditionalFormatting sqref="C7">
     <cfRule type="dataBar" priority="95">

</xml_diff>